<commit_message>
fixed problem with xpath
</commit_message>
<xml_diff>
--- a/services/sample.xlsx
+++ b/services/sample.xlsx
@@ -62,6 +62,24 @@
   </si>
   <si>
     <t>/html/body/div[1]/div/div[3]/div[1]/div/div[2]/div[3]/div/div[2]/div/div/div/div[1]/div/div[1]/div/div/div/span/span/span[1]</t>
+  </si>
+  <si>
+    <t>пылесос</t>
+  </si>
+  <si>
+    <t>https://uz.ozon.com/product/pylesos-vertikalnyy-besprovodnoy-futula-v8-belyy-vysokaya-moshchnost-v-9500pa-turbo-shchetka-s-1348678583/?_bctx=CAYQ-98y&amp;at=x6tPEj4LZhgAGLP1TY887Q7Cn9w2xOc502K98UnkLQj6</t>
+  </si>
+  <si>
+    <t>//*[@id="layoutPage"]/div[1]/div[3]/div[3]/div[2]/div/div/div[1]/div[2]/div/div[1]/div/div/div[1]/div/div[1]/div[1]/span[1]</t>
+  </si>
+  <si>
+    <t>сумка</t>
+  </si>
+  <si>
+    <t>https://aliexpress.ru/item/1005008688882796.html?spm=a2g2w.home.3.1.139f5586h1RuUJ&amp;mixer_rcmd_bucket_id=aerabtestalgoRecommendAbV2_testRankingFairPriceMerged&amp;ru_algo_pv_id=5f2048-ade163-e7d317-9725ba-1744909200&amp;scenario=aerMediaKitSegments&amp;spmC=homepage_main_shelf_pc&amp;spmD=3&amp;traffic_source=recommendation&amp;type_rcmd=core&amp;sku_id=12000046251455202</t>
+  </si>
+  <si>
+    <t>//*[@id="__aer_root__"]/div/div[8]/div[2]/div[4]/div/div[1]/div[1]/div/div[1]/div/div/div[2]</t>
   </si>
 </sst>
 </file>
@@ -396,8 +414,8 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A6">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -462,6 +480,28 @@
         <v>14</v>
       </c>
     </row>
+    <row r="6" ht="210">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" ht="165">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>